<commit_message>
Allow WaterOilGas construction for two-phase problems
Also fix leftover bugs related to kroend API change for factory, and
leftover refactoring for tests
</commit_message>
<xml_diff>
--- a/tests/data/scal-pc-input-example.xlsx
+++ b/tests/data/scal-pc-input-example.xlsx
@@ -5,106 +5,114 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="relperm" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
-  <si>
-    <t>SATNUM</t>
-  </si>
-  <si>
-    <t>CASE</t>
-  </si>
-  <si>
-    <t>sorw</t>
-  </si>
-  <si>
-    <t>swl</t>
-  </si>
-  <si>
-    <t>krwend</t>
-  </si>
-  <si>
-    <t>Lw</t>
-  </si>
-  <si>
-    <t>Ew</t>
-  </si>
-  <si>
-    <t>Tw</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Eow</t>
-  </si>
-  <si>
-    <t>Tow</t>
-  </si>
-  <si>
-    <t>Lg</t>
-  </si>
-  <si>
-    <t>Eg</t>
-  </si>
-  <si>
-    <t>Tg</t>
-  </si>
-  <si>
-    <t>Log</t>
-  </si>
-  <si>
-    <t>Eog</t>
-  </si>
-  <si>
-    <t>Tog</t>
-  </si>
-  <si>
-    <t>sorg</t>
-  </si>
-  <si>
-    <t>sgcr</t>
-  </si>
-  <si>
-    <t>krgend</t>
-  </si>
-  <si>
-    <t>kroend</t>
-  </si>
-  <si>
-    <t>swirr</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>poro_ref</t>
-  </si>
-  <si>
-    <t>perm_ref</t>
-  </si>
-  <si>
-    <t>drho</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>high</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+  <si>
+    <t xml:space="preserve">SATNUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sorw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krwend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sorg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sgcr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krgend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krogend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krowend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swirr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poro_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perm_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
   </si>
 </sst>
 </file>
@@ -112,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -187,12 +195,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -202,17 +210,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA11" activeCellId="0" sqref="AA11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.70918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,13 +303,16 @@
       <c r="AA1" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0.12</v>
@@ -363,21 +372,24 @@
         <v>1</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W2" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X2" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="Y2" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Z2" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="AA2" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AB2" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -386,7 +398,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.19</v>
@@ -446,21 +458,24 @@
         <v>1</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X3" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="Y3" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Z3" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="AA3" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AB3" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -469,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.22</v>
@@ -529,21 +544,24 @@
         <v>1</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W4" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X4" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="Y4" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Z4" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="AA4" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AB4" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -552,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0.14</v>
@@ -612,21 +630,24 @@
         <v>1</v>
       </c>
       <c r="V5" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W5" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X5" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X5" s="0" t="n">
+      <c r="Y5" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y5" s="0" t="n">
+      <c r="Z5" s="0" t="n">
         <v>0.18</v>
       </c>
-      <c r="Z5" s="0" t="n">
-        <v>300</v>
-      </c>
       <c r="AA5" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="AB5" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -635,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0.19</v>
@@ -695,21 +716,24 @@
         <v>1</v>
       </c>
       <c r="V6" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W6" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X6" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X6" s="0" t="n">
+      <c r="Y6" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y6" s="0" t="n">
+      <c r="Z6" s="0" t="n">
         <v>0.18</v>
       </c>
-      <c r="Z6" s="0" t="n">
-        <v>300</v>
-      </c>
       <c r="AA6" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="AB6" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -718,7 +742,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0.23</v>
@@ -778,21 +802,24 @@
         <v>1</v>
       </c>
       <c r="V7" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W7" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X7" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X7" s="0" t="n">
+      <c r="Y7" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y7" s="0" t="n">
+      <c r="Z7" s="0" t="n">
         <v>0.18</v>
       </c>
-      <c r="Z7" s="0" t="n">
-        <v>300</v>
-      </c>
       <c r="AA7" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="AB7" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -801,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0.13</v>
@@ -861,21 +888,24 @@
         <v>1</v>
       </c>
       <c r="V8" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W8" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X8" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X8" s="0" t="n">
+      <c r="Y8" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y8" s="0" t="n">
+      <c r="Z8" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="Z8" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="AA8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -884,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0.18</v>
@@ -944,21 +974,24 @@
         <v>1</v>
       </c>
       <c r="V9" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W9" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X9" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X9" s="0" t="n">
+      <c r="Y9" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y9" s="0" t="n">
+      <c r="Z9" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="Z9" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="AA9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="0" t="n">
         <v>300</v>
       </c>
     </row>
@@ -967,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0.21</v>
@@ -1027,28 +1060,31 @@
         <v>1</v>
       </c>
       <c r="V10" s="0" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W10" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X10" s="0" t="n">
         <v>0.321</v>
       </c>
-      <c r="X10" s="0" t="n">
+      <c r="Y10" s="0" t="n">
         <v>-1.283</v>
       </c>
-      <c r="Y10" s="0" t="n">
+      <c r="Z10" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="Z10" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="AA10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="0" t="n">
         <v>300</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>